<commit_message>
updated bondportfolio & scraping
</commit_message>
<xml_diff>
--- a/portfolio_obligacje.xlsx
+++ b/portfolio_obligacje.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -644,6 +644,52 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ARH0227</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Deweloper nieruchomości</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>101.62</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2025-01-07</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>KRI1025</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Zarządzanie wierzytelnościami</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>99.3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-01-07</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>